<commit_message>
Test-8 for tree (this year, MSE&MAPE)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-8.xlsx
+++ b/migforecasting/underground/test-8.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NextYear" sheetId="1" r:id="rId1"/>
+    <sheet name="ThisYear" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
   <si>
     <t>test size 20%</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>Random Forest-100 (citiesdataset-NY-4.csv) - next year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-2.csv) - this year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-DCor-3.csv) - this year</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-DCor-4.csv) - this year</t>
   </si>
 </sst>
 </file>
@@ -402,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:X58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -3215,4 +3225,2279 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:U58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="R63" sqref="R63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="18" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.2056791044918189</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.2729879855922368</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.04854709757751</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5.2491482331018018</v>
+      </c>
+      <c r="N6" s="2">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>9.1196311480614453E-4</v>
+      </c>
+      <c r="P6" s="4">
+        <v>5.8380202018514724E-3</v>
+      </c>
+      <c r="S6" s="2">
+        <v>1</v>
+      </c>
+      <c r="T6" s="4">
+        <v>9.7562966794317407E-4</v>
+      </c>
+      <c r="U6" s="4">
+        <v>5.948574401856018E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f>C6+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.99795762614404582</v>
+      </c>
+      <c r="E7" s="3">
+        <v>3.3400541455661759</v>
+      </c>
+      <c r="H7" s="2">
+        <f>H6+1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.081963010604972</v>
+      </c>
+      <c r="J7" s="3">
+        <v>3.7411515559598172</v>
+      </c>
+      <c r="N7" s="2">
+        <f>N6+1</f>
+        <v>2</v>
+      </c>
+      <c r="O7" s="4">
+        <v>1.0022162063098019E-3</v>
+      </c>
+      <c r="P7" s="4">
+        <v>5.3046415388013123E-3</v>
+      </c>
+      <c r="S7" s="2">
+        <f>S6+1</f>
+        <v>2</v>
+      </c>
+      <c r="T7" s="4">
+        <v>9.6271959322012722E-4</v>
+      </c>
+      <c r="U7" s="4">
+        <v>5.1389476994813509E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C55" si="0">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.13311698930376</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4.4462560975719221</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:H55" si="1">H7+1</f>
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.90960273956698701</v>
+      </c>
+      <c r="J8" s="3">
+        <v>4.6560839302902206</v>
+      </c>
+      <c r="N8" s="2">
+        <f t="shared" ref="N8:N55" si="2">N7+1</f>
+        <v>3</v>
+      </c>
+      <c r="O8" s="4">
+        <v>9.5276356433865287E-4</v>
+      </c>
+      <c r="P8" s="4">
+        <v>6.0639691734625956E-3</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" ref="S8:S55" si="3">S7+1</f>
+        <v>3</v>
+      </c>
+      <c r="T8" s="4">
+        <v>9.2000838219667485E-4</v>
+      </c>
+      <c r="U8" s="4">
+        <v>6.3343338363778482E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.125196249673893</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3.047146786999464</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.94883007455512802</v>
+      </c>
+      <c r="J9" s="3">
+        <v>5.4951337352194463</v>
+      </c>
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O9" s="4">
+        <v>8.9050104018420246E-4</v>
+      </c>
+      <c r="P9" s="4">
+        <v>7.0182112751593449E-3</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="T9" s="4">
+        <v>8.5737681545407338E-4</v>
+      </c>
+      <c r="U9" s="4">
+        <v>6.2843589567059552E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.94034876774283982</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.3256141378915798</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.177911562274105</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3.56209363188789</v>
+      </c>
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O10" s="4">
+        <v>8.7345378802373736E-4</v>
+      </c>
+      <c r="P10" s="4">
+        <v>8.8120279857618142E-3</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="T10" s="4">
+        <v>8.8515985919139148E-4</v>
+      </c>
+      <c r="U10" s="4">
+        <v>6.2120861769081239E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.0121474857262169</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5.0935257716333666</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.193973775332446</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2.484513562654155</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O11" s="4">
+        <v>9.5959056731180362E-4</v>
+      </c>
+      <c r="P11" s="4">
+        <v>5.8195493641756014E-3</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="T11" s="4">
+        <v>8.6409116897172289E-4</v>
+      </c>
+      <c r="U11" s="4">
+        <v>7.0624054853749858E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>1.0215708125950289</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4.6239216862370558</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.116102429877541</v>
+      </c>
+      <c r="J12" s="3">
+        <v>3.1912487594441412</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O12" s="4">
+        <v>1.000602112469183E-3</v>
+      </c>
+      <c r="P12" s="4">
+        <v>4.6894207913342539E-3</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="T12" s="4">
+        <v>8.8247840874564553E-4</v>
+      </c>
+      <c r="U12" s="4">
+        <v>6.5283610097444846E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.138917364969726</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.9544372342178828</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1.0219747309426219</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3.3256743762829002</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O13" s="4">
+        <v>8.97539958757951E-4</v>
+      </c>
+      <c r="P13" s="4">
+        <v>7.210461423343072E-3</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="T13" s="4">
+        <v>9.4659135001290884E-4</v>
+      </c>
+      <c r="U13" s="4">
+        <v>6.5726789659504986E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.0570581444786731</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2.5812904422824481</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.2025616865773721</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3.0544025853016028</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O14" s="4">
+        <v>9.3313014996185034E-4</v>
+      </c>
+      <c r="P14" s="4">
+        <v>6.6563622281744818E-3</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="T14" s="4">
+        <v>8.966891120511264E-4</v>
+      </c>
+      <c r="U14" s="4">
+        <v>7.1414561938690562E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1.2117980735284719</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.677596723500917</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1.1420348646711249</v>
+      </c>
+      <c r="J15" s="3">
+        <v>2.9223250310623521</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O15" s="4">
+        <v>9.2448569269220173E-4</v>
+      </c>
+      <c r="P15" s="4">
+        <v>5.5713613729078022E-3</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="T15" s="4">
+        <v>8.8667217595551093E-4</v>
+      </c>
+      <c r="U15" s="4">
+        <v>7.0149249675992929E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1.5252678619409561</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2.0949053100808008</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1.266601814966287</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.997425302332581</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O16" s="4">
+        <v>9.7813343192992342E-4</v>
+      </c>
+      <c r="P16" s="4">
+        <v>5.588069698938684E-3</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="T16" s="4">
+        <v>9.2578829671331167E-4</v>
+      </c>
+      <c r="U16" s="4">
+        <v>7.0939587578619399E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1.1896217616969209</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2.2609062125685142</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1.135157721188246</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.989252121792872</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O17" s="4">
+        <v>9.3864640250855124E-4</v>
+      </c>
+      <c r="P17" s="4">
+        <v>6.232337910902966E-3</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="T17" s="4">
+        <v>9.6609012092821261E-4</v>
+      </c>
+      <c r="U17" s="4">
+        <v>5.3214034414730462E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1.3086360885859349</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1.851207611589089</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1.1416724432433041</v>
+      </c>
+      <c r="J18" s="3">
+        <v>2.4615007577166299</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O18" s="4">
+        <v>8.1087155764451022E-4</v>
+      </c>
+      <c r="P18" s="4">
+        <v>8.1944715297911658E-3</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="T18" s="4">
+        <v>9.7620247155609638E-4</v>
+      </c>
+      <c r="U18" s="4">
+        <v>5.5615101764410471E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1.077026451559286</v>
+      </c>
+      <c r="E19" s="3">
+        <v>4.1530368143786029</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1.3424745531351669</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1.691970434666527</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O19" s="4">
+        <v>9.0590697593961379E-4</v>
+      </c>
+      <c r="P19" s="4">
+        <v>7.593555244641545E-3</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="T19" s="4">
+        <v>9.4143633875363065E-4</v>
+      </c>
+      <c r="U19" s="4">
+        <v>5.7074028064523106E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1.356206693529314</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1.839396885268415</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.1756871075292159</v>
+      </c>
+      <c r="J20" s="3">
+        <v>2.5371716218952689</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O20" s="4">
+        <v>9.0557647837213873E-4</v>
+      </c>
+      <c r="P20" s="4">
+        <v>7.5461846756831909E-3</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="T20" s="4">
+        <v>9.0774977429108992E-4</v>
+      </c>
+      <c r="U20" s="4">
+        <v>4.8187372814528289E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1.1900963614755851</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2.187063856021787</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1.064059751567404</v>
+      </c>
+      <c r="J21" s="3">
+        <v>2.7081907784243748</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O21" s="4">
+        <v>9.970750667908678E-4</v>
+      </c>
+      <c r="P21" s="4">
+        <v>4.7412430524547081E-3</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="T21" s="4">
+        <v>8.5174503392551149E-4</v>
+      </c>
+      <c r="U21" s="4">
+        <v>7.3026973870876947E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1.08526160831916</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1.60004595633669</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1.208471139652479</v>
+      </c>
+      <c r="J22" s="3">
+        <v>2.2380010540921922</v>
+      </c>
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O22" s="4">
+        <v>8.8527316283143595E-4</v>
+      </c>
+      <c r="P22" s="4">
+        <v>7.3950155175083561E-3</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="T22" s="4">
+        <v>8.9685830484820186E-4</v>
+      </c>
+      <c r="U22" s="4">
+        <v>5.9198496629323024E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.98063972528183418</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4.0375333828575197</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1.0647901638598469</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1.9496790221035001</v>
+      </c>
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O23" s="4">
+        <v>8.7271559401397964E-4</v>
+      </c>
+      <c r="P23" s="4">
+        <v>6.4661265226357368E-3</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="T23" s="4">
+        <v>9.9410276508855649E-4</v>
+      </c>
+      <c r="U23" s="4">
+        <v>4.388694708554324E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1.247853113988759</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1.7883271602324831</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1.100162787972101</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1.8466822242386749</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O24" s="4">
+        <v>9.535531562039275E-4</v>
+      </c>
+      <c r="P24" s="4">
+        <v>5.265783078721299E-3</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="T24" s="4">
+        <v>9.3353952901907675E-4</v>
+      </c>
+      <c r="U24" s="4">
+        <v>6.9197808076210381E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1.3026846083723591</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2.7567520245772501</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I25" s="3">
+        <v>1.0695550505199409</v>
+      </c>
+      <c r="J25" s="3">
+        <v>2.2371729467195651</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O25" s="4">
+        <v>9.7794115955868177E-4</v>
+      </c>
+      <c r="P25" s="4">
+        <v>5.2613637433965516E-3</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="T25" s="4">
+        <v>9.4325787723261324E-4</v>
+      </c>
+      <c r="U25" s="4">
+        <v>4.9712710900598357E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1.099241135447669</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2.4795267418455089</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I26" s="3">
+        <v>1.260967676385758</v>
+      </c>
+      <c r="J26" s="3">
+        <v>2.3157174825952969</v>
+      </c>
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O26" s="4">
+        <v>9.0016825812679264E-4</v>
+      </c>
+      <c r="P26" s="4">
+        <v>6.2060187817966489E-3</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="T26" s="4">
+        <v>8.3062838283077471E-4</v>
+      </c>
+      <c r="U26" s="4">
+        <v>9.071915143186067E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1.285968036394874</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3.121608480448121</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1.3904250659958539</v>
+      </c>
+      <c r="J27" s="3">
+        <v>2.2708062737391428</v>
+      </c>
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O27" s="4">
+        <v>1.015241755845895E-3</v>
+      </c>
+      <c r="P27" s="4">
+        <v>4.4788025287490138E-3</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="T27" s="4">
+        <v>8.6384148863865554E-4</v>
+      </c>
+      <c r="U27" s="4">
+        <v>6.5793479230795964E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1.1904958824152601</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2.2181372187220778</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1.0245423440047501</v>
+      </c>
+      <c r="J28" s="3">
+        <v>3.4543723593717388</v>
+      </c>
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O28" s="4">
+        <v>9.2899420333204493E-4</v>
+      </c>
+      <c r="P28" s="4">
+        <v>5.5947557613445836E-3</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="T28" s="4">
+        <v>8.8400308986118117E-4</v>
+      </c>
+      <c r="U28" s="4">
+        <v>6.2922129605074541E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.8998473243361742</v>
+      </c>
+      <c r="E29" s="3">
+        <v>7.09467169486771</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.95063792958139082</v>
+      </c>
+      <c r="J29" s="3">
+        <v>3.370245899068812</v>
+      </c>
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O29" s="4">
+        <v>9.4393048004325661E-4</v>
+      </c>
+      <c r="P29" s="4">
+        <v>5.3743688896886153E-3</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="T29" s="4">
+        <v>8.6566922072455691E-4</v>
+      </c>
+      <c r="U29" s="4">
+        <v>7.3814537120111962E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>1.468253258723812</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2.0598754398207682</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1.2145234791359141</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2.200421304710757</v>
+      </c>
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O30" s="4">
+        <v>7.7791704414868518E-4</v>
+      </c>
+      <c r="P30" s="4">
+        <v>1.0112245780850661E-2</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="T30" s="4">
+        <v>8.930609782073813E-4</v>
+      </c>
+      <c r="U30" s="4">
+        <v>6.4544850342400277E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>1.2405468639603969</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2.2424909217316151</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.92510905557097678</v>
+      </c>
+      <c r="J31" s="3">
+        <v>4.5621490728748482</v>
+      </c>
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O31" s="4">
+        <v>8.1101238271637655E-4</v>
+      </c>
+      <c r="P31" s="4">
+        <v>9.3658771157432673E-3</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="T31" s="4">
+        <v>8.8504514025191305E-4</v>
+      </c>
+      <c r="U31" s="4">
+        <v>5.6643246427666803E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1.320821067296722</v>
+      </c>
+      <c r="E32" s="3">
+        <v>2.608599231783272</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I32" s="3">
+        <v>1.131013422886038</v>
+      </c>
+      <c r="J32" s="3">
+        <v>2.601848605915936</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O32" s="4">
+        <v>1.0162481881235651E-3</v>
+      </c>
+      <c r="P32" s="4">
+        <v>6.8972753484131963E-3</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="T32" s="4">
+        <v>9.6721814599834042E-4</v>
+      </c>
+      <c r="U32" s="4">
+        <v>4.8287346966646898E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1.2043568008466421</v>
+      </c>
+      <c r="E33" s="3">
+        <v>2.328319183134639</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1.187154137526842</v>
+      </c>
+      <c r="J33" s="3">
+        <v>1.413921085578818</v>
+      </c>
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O33" s="4">
+        <v>9.3439847932420329E-4</v>
+      </c>
+      <c r="P33" s="4">
+        <v>6.3234373070772372E-3</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="T33" s="4">
+        <v>8.3460530349287957E-4</v>
+      </c>
+      <c r="U33" s="4">
+        <v>8.3762950912805688E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>1.1481534644030471</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1.9602978792595189</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0.95652070242509213</v>
+      </c>
+      <c r="J34" s="3">
+        <v>4.2264652472169093</v>
+      </c>
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O34" s="4">
+        <v>9.0069347789100741E-4</v>
+      </c>
+      <c r="P34" s="4">
+        <v>6.9893486861439952E-3</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="T34" s="4">
+        <v>8.5746034586152507E-4</v>
+      </c>
+      <c r="U34" s="4">
+        <v>8.1692502147757244E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1.191427924979201</v>
+      </c>
+      <c r="E35" s="3">
+        <v>2.886479600721982</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1.311321835933146</v>
+      </c>
+      <c r="J35" s="3">
+        <v>1.8946445771393361</v>
+      </c>
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O35" s="4">
+        <v>9.7227946116014159E-4</v>
+      </c>
+      <c r="P35" s="4">
+        <v>6.8224504642190997E-3</v>
+      </c>
+      <c r="S35" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="T35" s="4">
+        <v>8.5766469141243941E-4</v>
+      </c>
+      <c r="U35" s="4">
+        <v>6.8074496380397193E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="3">
+        <v>1.397398083734074</v>
+      </c>
+      <c r="E36" s="3">
+        <v>2.0370402508698948</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1.0822256650930651</v>
+      </c>
+      <c r="J36" s="3">
+        <v>1.734167442362506</v>
+      </c>
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O36" s="4">
+        <v>9.2384478130150564E-4</v>
+      </c>
+      <c r="P36" s="4">
+        <v>5.835685680643965E-3</v>
+      </c>
+      <c r="S36" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="T36" s="4">
+        <v>8.4559578797336222E-4</v>
+      </c>
+      <c r="U36" s="4">
+        <v>7.738344592897935E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>1.063087104993955</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2.7495281753048468</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0.99232824052919355</v>
+      </c>
+      <c r="J37" s="3">
+        <v>5.2872548811506546</v>
+      </c>
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O37" s="4">
+        <v>8.8436240981511953E-4</v>
+      </c>
+      <c r="P37" s="4">
+        <v>5.7945371857014462E-3</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="T37" s="4">
+        <v>8.8067846815377256E-4</v>
+      </c>
+      <c r="U37" s="4">
+        <v>7.2326310783706977E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1.208349551353872</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2.560692724154114</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1.2278125694466731</v>
+      </c>
+      <c r="J38" s="3">
+        <v>2.5504690213809238</v>
+      </c>
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O38" s="4">
+        <v>8.8315389679396485E-4</v>
+      </c>
+      <c r="P38" s="4">
+        <v>5.1902964772459472E-3</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="T38" s="4">
+        <v>8.6025214986808099E-4</v>
+      </c>
+      <c r="U38" s="4">
+        <v>7.657562701608822E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D39" s="3">
+        <v>1.0376609122206899</v>
+      </c>
+      <c r="E39" s="3">
+        <v>3.5619617170987632</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I39" s="3">
+        <v>1.0350825530047401</v>
+      </c>
+      <c r="J39" s="3">
+        <v>3.8194899081236069</v>
+      </c>
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O39" s="4">
+        <v>9.4052651053605832E-4</v>
+      </c>
+      <c r="P39" s="4">
+        <v>6.4219400244938246E-3</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="T39" s="4">
+        <v>1.0076951699113791E-3</v>
+      </c>
+      <c r="U39" s="4">
+        <v>4.8019055077945646E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="3">
+        <v>1.347269213052021</v>
+      </c>
+      <c r="E40" s="3">
+        <v>2.4589019659816072</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1.0254964552134569</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1.6325351112974851</v>
+      </c>
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O40" s="4">
+        <v>8.1209128390349677E-4</v>
+      </c>
+      <c r="P40" s="4">
+        <v>8.2393522462164675E-3</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="T40" s="4">
+        <v>9.6046926400855984E-4</v>
+      </c>
+      <c r="U40" s="4">
+        <v>4.7365955958676804E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1.08397405059351</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1.867224051310461</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I41" s="3">
+        <v>1.0581445794149089</v>
+      </c>
+      <c r="J41" s="3">
+        <v>3.2728950796441838</v>
+      </c>
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O41" s="4">
+        <v>8.7365716151930164E-4</v>
+      </c>
+      <c r="P41" s="4">
+        <v>6.052312985222361E-3</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="T41" s="4">
+        <v>9.3562261787399079E-4</v>
+      </c>
+      <c r="U41" s="4">
+        <v>6.0364714180354681E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1.1673806908197391</v>
+      </c>
+      <c r="E42" s="3">
+        <v>2.16408464525334</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I42" s="3">
+        <v>1.215137387328705</v>
+      </c>
+      <c r="J42" s="3">
+        <v>3.687813643466352</v>
+      </c>
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O42" s="4">
+        <v>9.1587946043700783E-4</v>
+      </c>
+      <c r="P42" s="4">
+        <v>5.2451061850339051E-3</v>
+      </c>
+      <c r="S42" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="T42" s="4">
+        <v>9.9685941864207771E-4</v>
+      </c>
+      <c r="U42" s="4">
+        <v>5.4778078159888038E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D43" s="3">
+        <v>1.1131675225327931</v>
+      </c>
+      <c r="E43" s="3">
+        <v>3.0341103181973459</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1.035912241533407</v>
+      </c>
+      <c r="J43" s="3">
+        <v>5.5497685225395932</v>
+      </c>
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O43" s="4">
+        <v>8.9343627504547311E-4</v>
+      </c>
+      <c r="P43" s="4">
+        <v>5.8037782182251479E-3</v>
+      </c>
+      <c r="S43" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="T43" s="4">
+        <v>9.5259560533634581E-4</v>
+      </c>
+      <c r="U43" s="4">
+        <v>5.4982134349418257E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1.317787310340967</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1.9015016274806491</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I44" s="3">
+        <v>1.0871365580811829</v>
+      </c>
+      <c r="J44" s="3">
+        <v>2.2065805048059488</v>
+      </c>
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O44" s="4">
+        <v>9.7551464150883176E-4</v>
+      </c>
+      <c r="P44" s="4">
+        <v>6.2514298095603044E-3</v>
+      </c>
+      <c r="S44" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="T44" s="4">
+        <v>8.5794860729040804E-4</v>
+      </c>
+      <c r="U44" s="4">
+        <v>7.4605402781944257E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.85357227491798637</v>
+      </c>
+      <c r="E45" s="3">
+        <v>6.7284237569665981</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1.2309793436459591</v>
+      </c>
+      <c r="J45" s="3">
+        <v>1.9432554161158611</v>
+      </c>
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O45" s="4">
+        <v>8.4771113559812129E-4</v>
+      </c>
+      <c r="P45" s="4">
+        <v>8.3069433673470718E-3</v>
+      </c>
+      <c r="S45" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="T45" s="4">
+        <v>9.1575710286213711E-4</v>
+      </c>
+      <c r="U45" s="4">
+        <v>6.5385610657263376E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1.2667193803499599</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2.5562570431765161</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1.057019693230056</v>
+      </c>
+      <c r="J46" s="3">
+        <v>2.3985116541482818</v>
+      </c>
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O46" s="4">
+        <v>8.781766987495433E-4</v>
+      </c>
+      <c r="P46" s="4">
+        <v>6.53197148873741E-3</v>
+      </c>
+      <c r="S46" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="T46" s="4">
+        <v>8.8206561441162533E-4</v>
+      </c>
+      <c r="U46" s="4">
+        <v>6.485421815057367E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1.2665557089188391</v>
+      </c>
+      <c r="E47" s="3">
+        <v>2.3333529682993772</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1.440752303788071</v>
+      </c>
+      <c r="J47" s="3">
+        <v>1.9994833187625149</v>
+      </c>
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O47" s="4">
+        <v>8.9820920089064729E-4</v>
+      </c>
+      <c r="P47" s="4">
+        <v>7.4229273020972814E-3</v>
+      </c>
+      <c r="S47" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="T47" s="4">
+        <v>8.4369921000908591E-4</v>
+      </c>
+      <c r="U47" s="4">
+        <v>7.2448262239702098E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1.1362498679997659</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2.5732707697016921</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1.240831619831464</v>
+      </c>
+      <c r="J48" s="3">
+        <v>3.3098403795640681</v>
+      </c>
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O48" s="4">
+        <v>9.0615864008485503E-4</v>
+      </c>
+      <c r="P48" s="4">
+        <v>5.9616225295558217E-3</v>
+      </c>
+      <c r="S48" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="T48" s="4">
+        <v>9.1842749853416337E-4</v>
+      </c>
+      <c r="U48" s="4">
+        <v>5.6569162905039114E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D49" s="3">
+        <v>1.043925586311016</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2.9588101316047331</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I49" s="3">
+        <v>1.1429978147108859</v>
+      </c>
+      <c r="J49" s="3">
+        <v>2.099810928474267</v>
+      </c>
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O49" s="4">
+        <v>8.951977412125368E-4</v>
+      </c>
+      <c r="P49" s="4">
+        <v>6.2963024719676257E-3</v>
+      </c>
+      <c r="S49" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="T49" s="4">
+        <v>8.7847327451849957E-4</v>
+      </c>
+      <c r="U49" s="4">
+        <v>5.5422496217548637E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1.1640722779636701</v>
+      </c>
+      <c r="E50" s="3">
+        <v>3.1516746441330592</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I50" s="3">
+        <v>1.0828044843601019</v>
+      </c>
+      <c r="J50" s="3">
+        <v>2.0248494981346332</v>
+      </c>
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O50" s="4">
+        <v>8.354892445129609E-4</v>
+      </c>
+      <c r="P50" s="4">
+        <v>7.7759996260347809E-3</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="T50" s="4">
+        <v>8.5825624421367094E-4</v>
+      </c>
+      <c r="U50" s="4">
+        <v>7.4497439866132399E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1.12677083333433</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1.876406953901137</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I51" s="3">
+        <v>1.3138326130491631</v>
+      </c>
+      <c r="J51" s="3">
+        <v>2.5315176985718</v>
+      </c>
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O51" s="4">
+        <v>9.9070051289274863E-4</v>
+      </c>
+      <c r="P51" s="4">
+        <v>4.8704509442503516E-3</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="T51" s="4">
+        <v>9.0516141809272453E-4</v>
+      </c>
+      <c r="U51" s="4">
+        <v>6.1013390343725602E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.88592487970189449</v>
+      </c>
+      <c r="E52" s="3">
+        <v>6.5971396548057202</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0.99627707958043299</v>
+      </c>
+      <c r="J52" s="3">
+        <v>3.822675038453148</v>
+      </c>
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O52" s="4">
+        <v>8.1560905800920152E-4</v>
+      </c>
+      <c r="P52" s="4">
+        <v>7.5256056845682869E-3</v>
+      </c>
+      <c r="S52" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="T52" s="4">
+        <v>9.6926510214619317E-4</v>
+      </c>
+      <c r="U52" s="4">
+        <v>6.1114804861822046E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1.1628513982455959</v>
+      </c>
+      <c r="E53" s="3">
+        <v>2.263982885489348</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I53" s="3">
+        <v>1.086707237870292</v>
+      </c>
+      <c r="J53" s="3">
+        <v>2.521087701229408</v>
+      </c>
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O53" s="4">
+        <v>7.6591156694121021E-4</v>
+      </c>
+      <c r="P53" s="4">
+        <v>1.248598281393873E-2</v>
+      </c>
+      <c r="S53" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="T53" s="4">
+        <v>9.2108080371374617E-4</v>
+      </c>
+      <c r="U53" s="4">
+        <v>6.8181947582650632E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D54" s="3">
+        <v>1.3763428007271949</v>
+      </c>
+      <c r="E54" s="3">
+        <v>2.3741232428182348</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I54" s="3">
+        <v>1.1127641774852719</v>
+      </c>
+      <c r="J54" s="3">
+        <v>4.5897155960875091</v>
+      </c>
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O54" s="4">
+        <v>8.7947686879334371E-4</v>
+      </c>
+      <c r="P54" s="4">
+        <v>7.0561020580377802E-3</v>
+      </c>
+      <c r="S54" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="T54" s="4">
+        <v>9.3022559007159718E-4</v>
+      </c>
+      <c r="U54" s="4">
+        <v>5.5652675940663331E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="3">
+        <v>1.274361759814852</v>
+      </c>
+      <c r="E55" s="3">
+        <v>2.9399033213789258</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I55" s="3">
+        <v>1.066232684288891</v>
+      </c>
+      <c r="J55" s="3">
+        <v>2.9689675165150708</v>
+      </c>
+      <c r="N55" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O55" s="4">
+        <v>9.8520832375428337E-4</v>
+      </c>
+      <c r="P55" s="4">
+        <v>6.1705349126849919E-3</v>
+      </c>
+      <c r="S55" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="T55" s="4">
+        <v>8.5830115698479724E-4</v>
+      </c>
+      <c r="U55" s="4">
+        <v>7.0082579532607034E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" s="3">
+        <f>AVERAGE(D6:D55)</f>
+        <v>1.1689923572027021</v>
+      </c>
+      <c r="E57" s="3">
+        <f>AVERAGE(E6:E55)</f>
+        <v>2.9724080693133152</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I57" s="3">
+        <f>AVERAGE(I6:I55)</f>
+        <v>1.1258965091309094</v>
+      </c>
+      <c r="J57" s="3">
+        <f>AVERAGE(J6:J55)</f>
+        <v>2.9520020486845184</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O57" s="4">
+        <f>AVERAGE(O6:O55)</f>
+        <v>9.1146276647322694E-4</v>
+      </c>
+      <c r="P57" s="4">
+        <f>AVERAGE(P6:P55)</f>
+        <v>6.6134327801047142E-3</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T57" s="4">
+        <f>AVERAGE(T6:T55)</f>
+        <v>9.0663627875989033E-4</v>
+      </c>
+      <c r="U57" s="4">
+        <f>AVERAGE(U6:U55)</f>
+        <v>6.3806246824765732E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="3">
+        <f>_xlfn.STDEV.S(D6:D55)</f>
+        <v>0.14528175160352255</v>
+      </c>
+      <c r="E58" s="3">
+        <f>_xlfn.STDEV.S(E6:E55)</f>
+        <v>1.3111645875663389</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I58" s="3">
+        <f>_xlfn.STDEV.S(I6:I55)</f>
+        <v>0.11957966032631687</v>
+      </c>
+      <c r="J58" s="3">
+        <f>_xlfn.STDEV.S(J6:J55)</f>
+        <v>1.0897208947427011</v>
+      </c>
+      <c r="N58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O58" s="4">
+        <f>_xlfn.STDEV.S(O6:O55)</f>
+        <v>6.0997195610198861E-5</v>
+      </c>
+      <c r="P58" s="4">
+        <f>_xlfn.STDEV.S(P6:P55)</f>
+        <v>1.4796067294317152E-3</v>
+      </c>
+      <c r="S58" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T58" s="4">
+        <f>_xlfn.STDEV.S(T6:T55)</f>
+        <v>4.7473645868940996E-5</v>
+      </c>
+      <c r="U58" s="4">
+        <f>_xlfn.STDEV.S(U6:U55)</f>
+        <v>1.0220449389700865E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test-8 with plots (for nextyear)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-8.xlsx
+++ b/migforecasting/underground/test-8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NextYear" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t>test size 20%</t>
   </si>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>Random Forest-100 (citiesdataset-DCor-4.csv) - this year</t>
+  </si>
+  <si>
+    <t>train</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Без инфляции</t>
+  </si>
+  <si>
+    <t>С инфляцией</t>
+  </si>
+  <si>
+    <t>Долларовая норм.</t>
+  </si>
+  <si>
+    <t>Инфляционная норм.</t>
   </si>
 </sst>
 </file>
@@ -145,6 +163,3237 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400"/>
+              <a:t>Прогноз</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" baseline="0"/>
+              <a:t> следующего года (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>Mape)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Обучающая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$F$64:$G$64</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Без инфляции</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>С инфляцией</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$F$65:$G$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.0063219175999294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0845545000076726</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CAE7-4985-B9E2-119D4CFD2F16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Тестовая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$F$64:$G$64</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Без инфляции</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>С инфляцией</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$F$66:$G$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.0803250309981398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7726662858793261</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-CAE7-4985-B9E2-119D4CFD2F16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="745203471"/>
+        <c:axId val="745198895"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="745203471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="745198895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="745198895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="745203471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400"/>
+              <a:t>Прогноз</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" baseline="0"/>
+              <a:t> следующего года (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>MSE)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Обучающая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$O$64:$P$64</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Без инфляции</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>С инфляцией</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$O$65:$P$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.077633109209872E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8362063642017849E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B3EE-418B-869E-1F510ABD4E49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Тестовая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$O$64:$P$64</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Без инфляции</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>С инфляцией</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$O$66:$P$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.6087655833538114E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1840187082965866E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B3EE-418B-869E-1F510ABD4E49}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="745203471"/>
+        <c:axId val="745198895"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="745203471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="745198895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="745198895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="745203471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400"/>
+              <a:t>Прогноз</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" baseline="0"/>
+              <a:t> следующего года (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" baseline="0"/>
+              <a:t>MSE)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="150" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Обучающая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$Z$64:$AA$64</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Долларовая норм.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Инфляционная норм.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$Z$65:$AA$65</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.2303205306975915E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8362063642017849E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-39A2-46D6-A7EB-2FA7896A1C06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Тестовая выборка (сред.)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>NextYear!$Z$64:$AA$64</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Долларовая норм.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Инфляционная норм.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>NextYear!$Z$66:$AA$66</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.2951311551990999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.1840187082965866E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-39A2-46D6-A7EB-2FA7896A1C06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="745203471"/>
+        <c:axId val="745198895"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="745203471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="745198895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="745198895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="745203471"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>515471</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>90767</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>403410</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>67234</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>123265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>952498</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>99732</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>425824</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>392205</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>110937</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,10 +3659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:X58"/>
+  <dimension ref="C3:AA66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,7 +5992,7 @@
         <v>4.9458893262739924E-3</v>
       </c>
     </row>
-    <row r="49" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2795,7 +6044,7 @@
         <v>4.9076265266630031E-3</v>
       </c>
     </row>
-    <row r="50" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2847,7 +6096,7 @@
         <v>6.7260318587086636E-3</v>
       </c>
     </row>
-    <row r="51" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2899,7 +6148,7 @@
         <v>6.078230571874111E-3</v>
       </c>
     </row>
-    <row r="52" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2951,7 +6200,7 @@
         <v>6.7297088389440159E-3</v>
       </c>
     </row>
-    <row r="53" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -3003,7 +6252,7 @@
         <v>5.2509018697693846E-3</v>
       </c>
     </row>
-    <row r="54" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -3055,7 +6304,7 @@
         <v>5.3804233015057193E-3</v>
       </c>
     </row>
-    <row r="55" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C55" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -3107,7 +6356,7 @@
         <v>6.5708800098847973E-3</v>
       </c>
     </row>
-    <row r="57" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
@@ -3164,7 +6413,7 @@
         <v>6.1840187082965866E-3</v>
       </c>
     </row>
-    <row r="58" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:27" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
         <v>5</v>
       </c>
@@ -3221,9 +6470,88 @@
         <v>1.1520144499880896E-3</v>
       </c>
     </row>
+    <row r="64" spans="3:27" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" t="s">
+        <v>18</v>
+      </c>
+      <c r="O64" t="s">
+        <v>17</v>
+      </c>
+      <c r="P64" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1.0063219175999294</v>
+      </c>
+      <c r="G65" s="3">
+        <v>1.0845545000076726</v>
+      </c>
+      <c r="N65" t="s">
+        <v>15</v>
+      </c>
+      <c r="O65" s="4">
+        <v>1.077633109209872E-3</v>
+      </c>
+      <c r="P65" s="4">
+        <v>8.8362063642017849E-4</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z65" s="4">
+        <v>9.2303205306975915E-4</v>
+      </c>
+      <c r="AA65" s="4">
+        <v>8.8362063642017849E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="5:27" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="3">
+        <v>3.0803250309981398</v>
+      </c>
+      <c r="G66" s="3">
+        <v>2.7726662858793261</v>
+      </c>
+      <c r="N66" t="s">
+        <v>16</v>
+      </c>
+      <c r="O66" s="4">
+        <v>7.6087655833538114E-3</v>
+      </c>
+      <c r="P66" s="4">
+        <v>6.1840187082965866E-3</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z66" s="4">
+        <v>6.2951311551990999E-3</v>
+      </c>
+      <c r="AA66" s="4">
+        <v>6.1840187082965866E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3231,7 +6559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="R63" sqref="R63"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Test-9 for tree (thisyear, nextyear)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/test-8.xlsx
+++ b/migforecasting/underground/test-8.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NextYear" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="22">
   <si>
     <t>test size 20%</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Инфляционная норм.</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (citiesdataset-Dcor-4.csv) - this year</t>
   </si>
 </sst>
 </file>
@@ -4737,7 +4740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AM66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V57" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AR64" sqref="AR64"/>
     </sheetView>
   </sheetViews>
@@ -7659,8 +7662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:U58"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="R63" sqref="R63"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7695,7 +7698,7 @@
       </c>
       <c r="E4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J4" s="1"/>
       <c r="N4" s="1" t="s">

</xml_diff>